<commit_message>
SQL Finish 1.2, 1.3, 1.4
</commit_message>
<xml_diff>
--- a/1.4-exercicio-optus/EXE.Modelagem_1.4.xlsx
+++ b/1.4-exercicio-optus/EXE.Modelagem_1.4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55119\Desktop\BDD_SQL\1.4-exercicio-optus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIC\Desktop\BANCO_DE_DADOS_SQL\1.4-exercicio-optus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E398F065-EDAC-4265-99C1-9CAE2FAB3BE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D6384-A4F5-424A-9832-8B118577C6EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F995D228-16D7-4DF1-AA11-B99B4483AEE0}"/>
   </bookViews>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEE39B7-564A-441F-B300-812237685F66}">
   <dimension ref="A2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>